<commit_message>
Basic Schedule with ADS
</commit_message>
<xml_diff>
--- a/mam.xlsx
+++ b/mam.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilbernard/localprojects/vipe_schedule_creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5ECBB4-A230-7C4B-9B94-BAC157833993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99882602-199A-4349-A350-0E853C5B409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{6A635D32-5842-0747-B336-5A4F3B85289E}"/>
+    <workbookView xWindow="12980" yWindow="30060" windowWidth="28040" windowHeight="16640" xr2:uid="{6A635D32-5842-0747-B336-5A4F3B85289E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>1. VIRTUAL AD INSERTION.mp4</t>
   </si>
@@ -90,6 +90,78 @@
   </si>
   <si>
     <t>00:05:01:22</t>
+  </si>
+  <si>
+    <t>BTVP1007</t>
+  </si>
+  <si>
+    <t>BTVP1008</t>
+  </si>
+  <si>
+    <t>BTVP1009</t>
+  </si>
+  <si>
+    <t>BTVP1010</t>
+  </si>
+  <si>
+    <t>BTVP1011</t>
+  </si>
+  <si>
+    <t>BTVP1012</t>
+  </si>
+  <si>
+    <t>BTVP1013</t>
+  </si>
+  <si>
+    <t>BTVP1014</t>
+  </si>
+  <si>
+    <t>BTVP1015</t>
+  </si>
+  <si>
+    <t>BTVP1016</t>
+  </si>
+  <si>
+    <t>BTVP1017</t>
+  </si>
+  <si>
+    <t>BTVP1018</t>
+  </si>
+  <si>
+    <t>Ology</t>
+  </si>
+  <si>
+    <t>XDCAM50</t>
+  </si>
+  <si>
+    <t>AVC100</t>
+  </si>
+  <si>
+    <t>AVC101</t>
+  </si>
+  <si>
+    <t>AVC102</t>
+  </si>
+  <si>
+    <t>AVC103</t>
+  </si>
+  <si>
+    <t>AVC104</t>
+  </si>
+  <si>
+    <t>AVC105</t>
+  </si>
+  <si>
+    <t>BT AD</t>
+  </si>
+  <si>
+    <t>00:02:23:00</t>
+  </si>
+  <si>
+    <t>00:00:50:22</t>
+  </si>
+  <si>
+    <t>00:01:01:03</t>
   </si>
 </sst>
 </file>
@@ -131,8 +203,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,15 +520,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F022A2E-531D-5C47-BFDA-98D5A476756F}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E7" sqref="E7:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -465,8 +538,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -476,8 +552,11 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -487,8 +566,11 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -498,8 +580,11 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -509,8 +594,11 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -519,6 +607,96 @@
       </c>
       <c r="E6" t="s">
         <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>